<commit_message>
working converter for title and menu, tested in crase
</commit_message>
<xml_diff>
--- a/input-ready/input-mkt-firm1.xlsx
+++ b/input-ready/input-mkt-firm1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabe/Documents/Gabe/myOther/CRASE/code/input-ready/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710D32DF-F64A-074D-A7E7-EB3C54CF10E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66F0909-5A37-DD48-8A8A-56BDFF2888E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12780" yWindow="-28300" windowWidth="17420" windowHeight="27600" xr2:uid="{572FEF65-569D-6441-82D7-91DDB4E912C7}"/>
+    <workbookView xWindow="-1980" yWindow="-27520" windowWidth="28800" windowHeight="17500" xr2:uid="{572FEF65-569D-6441-82D7-91DDB4E912C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing Plan" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Cornell</t>
   </si>
@@ -113,21 +113,6 @@
     <t>Season:</t>
   </si>
   <si>
-    <t>Steak</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Pasta</t>
-  </si>
-  <si>
-    <t>Wine</t>
-  </si>
-  <si>
-    <t>Spirits</t>
-  </si>
-  <si>
     <t>Filet</t>
   </si>
   <si>
@@ -140,9 +125,6 @@
     <t>Domestic</t>
   </si>
   <si>
-    <t>Top Shelf</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
@@ -156,6 +138,27 @@
   </si>
   <si>
     <t>Winter</t>
+  </si>
+  <si>
+    <t>STEAK</t>
+  </si>
+  <si>
+    <t>CHICKEN</t>
+  </si>
+  <si>
+    <t>PASTA</t>
+  </si>
+  <si>
+    <t>PIZZA</t>
+  </si>
+  <si>
+    <t>WINE</t>
+  </si>
+  <si>
+    <t>SPIRITS</t>
+  </si>
+  <si>
+    <t>Well</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +211,12 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -273,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -317,6 +326,16 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -327,9 +346,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -669,7 +685,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -699,12 +715,12 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="14"/>
       <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -720,7 +736,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -741,10 +757,10 @@
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="20"/>
       <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
@@ -754,17 +770,17 @@
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E10" s="10">
         <v>165</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H10" s="12">
         <v>1750</v>
@@ -773,19 +789,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16"/>
+    </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E12" s="10">
         <v>165</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H12" s="12">
         <v>1750</v>
@@ -794,19 +812,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+    </row>
     <row r="14" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="E14" s="10">
         <v>175</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H14" s="12">
         <v>1750</v>
@@ -815,19 +835,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16"/>
+    </row>
     <row r="16" spans="1:10" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>28</v>
+      <c r="A16" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E16" s="10">
         <v>150</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H16" s="12">
         <v>1750</v>
@@ -836,46 +858,50 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:12" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="16"/>
+    </row>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="E18" s="10">
         <v>15</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H18" s="12">
         <v>1750</v>
       </c>
       <c r="J18" s="13">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="16"/>
+    </row>
     <row r="20" spans="1:12" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>29</v>
+      <c r="A20" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E20" s="10">
         <v>4</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H20" s="12">
         <v>1750</v>
       </c>
       <c r="J20" s="13">
-        <v>6.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -902,16 +928,16 @@
       <c r="C27" s="13">
         <v>26</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
     </row>
     <row r="28" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="3"/>
@@ -920,16 +946,16 @@
       <c r="C29" s="13">
         <v>16.25</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -942,48 +968,48 @@
       <c r="C33" s="13">
         <v>1.25</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
     </row>
     <row r="34" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" s="12">
         <v>12000</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
     </row>
     <row r="36" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="12">
         <v>15000</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
     </row>
     <row r="38" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -998,10 +1024,10 @@
       <c r="C41" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="16"/>
+      <c r="F41" s="19"/>
       <c r="H41" s="7" t="s">
         <v>20</v>
       </c>
@@ -1026,7 +1052,7 @@
         <v>22</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>